<commit_message>
init all number exception
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -22,6 +22,7 @@
     <sheet name="1new" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="177">
   <si>
     <t xml:space="preserve">        &lt;item&gt;GMT-1&lt;/item&gt; </t>
   </si>
@@ -674,19 +675,48 @@
     <t>K1 &lt; K2 &amp;&amp;  K1 != K2</t>
   </si>
   <si>
-    <t>K1 &lt; K2 &amp;&amp;  K1 != K3</t>
-  </si>
-  <si>
-    <t>K1 &lt; K2 &amp;&amp;  K1 != K4</t>
-  </si>
-  <si>
-    <t>K1 &lt; K2 &amp;&amp;  K1 != K5</t>
-  </si>
-  <si>
-    <t>K1 &lt; K2 &amp;&amp;  K1 != K6</t>
-  </si>
-  <si>
     <t>K[55]</t>
+  </si>
+  <si>
+    <t>K1 &lt; K3 &amp;&amp;  K1 != K3</t>
+  </si>
+  <si>
+    <t>K1 &lt; K4 &amp;&amp;  K1 != K4</t>
+  </si>
+  <si>
+    <t>K1 &lt; K5 &amp;&amp;  K1 != K5</t>
+  </si>
+  <si>
+    <t>K1 &lt; K6 &amp;&amp;  K1 != K6</t>
+  </si>
+  <si>
+    <t>K[(jml prima-k1)]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">n = 0 ( </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> )</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -787,7 +817,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -803,6 +833,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1218,108 +1254,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1328,9 +1262,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1338,30 +1269,146 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="21" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1521,15 +1568,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>189672</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>877957</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1563,8 +1610,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2076450" y="2095500"/>
-          <a:ext cx="657225" cy="200025"/>
+          <a:off x="1904172" y="2517913"/>
+          <a:ext cx="688285" cy="180974"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1862,42 +1909,42 @@
   <sheetData>
     <row r="2" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="77"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="89"/>
     </row>
     <row r="4" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="78"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="92"/>
     </row>
     <row r="5" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="72"/>
+      <c r="E5" s="84"/>
       <c r="F5" s="64"/>
       <c r="G5" s="65"/>
-      <c r="H5" s="71" t="s">
+      <c r="H5" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="72"/>
+      <c r="I5" s="84"/>
     </row>
     <row r="6" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="73"/>
-      <c r="E6" s="74"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
       <c r="F6" s="64"/>
       <c r="G6" s="65"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="74"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="86"/>
     </row>
     <row r="7" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D7" s="66" t="s">
@@ -2158,23 +2205,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
     </row>
     <row r="2" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="83" t="s">
+      <c r="D2" s="95" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="97"/>
       <c r="I2" s="32"/>
       <c r="M2" s="24">
         <v>4814863028233940</v>
@@ -2184,13 +2231,13 @@
       <c r="C3" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="108" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="98"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="110"/>
       <c r="I3" s="32"/>
       <c r="M3" t="s">
         <v>92</v>
@@ -2198,55 +2245,55 @@
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4" s="4"/>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="98"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="110"/>
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C5" s="4"/>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="108" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="98"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="110"/>
       <c r="I5" s="32"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="108" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="98"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="110"/>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C7" s="4"/>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="108" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="97"/>
-      <c r="H7" s="98"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="110"/>
     </row>
     <row r="8" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="5"/>
-      <c r="D8" s="99" t="s">
+      <c r="D8" s="111" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="101"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="113"/>
       <c r="M8" t="s">
         <v>93</v>
       </c>
@@ -2255,13 +2302,13 @@
       <c r="C9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="82"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="94"/>
       <c r="M9" t="s">
         <v>94</v>
       </c>
@@ -2526,26 +2573,26 @@
       <c r="C21" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="95"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="107"/>
       <c r="I21" s="24"/>
     </row>
     <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="93" t="s">
+      <c r="D22" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="94"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="95"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="106"/>
+      <c r="H22" s="107"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
@@ -2622,25 +2669,25 @@
       <c r="C48" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="86" t="s">
+      <c r="D48" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="87"/>
-      <c r="H48" s="88"/>
+      <c r="E48" s="99"/>
+      <c r="F48" s="99"/>
+      <c r="G48" s="99"/>
+      <c r="H48" s="100"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="89" t="s">
+      <c r="D49" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="91"/>
+      <c r="E49" s="102"/>
+      <c r="F49" s="102"/>
+      <c r="G49" s="102"/>
+      <c r="H49" s="103"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="4" t="s">
@@ -2928,10 +2975,10 @@
       </c>
     </row>
     <row r="75" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F75" s="81" t="s">
+      <c r="F75" s="93" t="s">
         <v>118</v>
       </c>
-      <c r="G75" s="82"/>
+      <c r="G75" s="94"/>
       <c r="H75" s="38">
         <f>AVERAGE(H70:H74)</f>
         <v>120.4</v>
@@ -3992,22 +4039,22 @@
       <c r="D5" s="59">
         <v>0.45837962962962964</v>
       </c>
-      <c r="E5" s="103">
+      <c r="E5" s="115">
         <v>1</v>
       </c>
       <c r="F5" s="61">
         <v>0.25005787037037036</v>
       </c>
-      <c r="G5" s="103">
+      <c r="G5" s="115">
         <v>23</v>
       </c>
-      <c r="H5" s="103">
+      <c r="H5" s="115">
         <v>97</v>
       </c>
-      <c r="I5" s="103">
+      <c r="I5" s="115">
         <v>227</v>
       </c>
-      <c r="J5" s="103">
+      <c r="J5" s="115">
         <v>2</v>
       </c>
     </row>
@@ -4015,35 +4062,35 @@
       <c r="D6" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="104"/>
+      <c r="E6" s="116"/>
       <c r="F6" s="55" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116"/>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D7" s="59">
         <v>0.46186342592592594</v>
       </c>
-      <c r="E7" s="103">
+      <c r="E7" s="115">
         <v>2</v>
       </c>
       <c r="F7" s="61">
         <v>0.25354166666666667</v>
       </c>
-      <c r="G7" s="103">
+      <c r="G7" s="115">
         <v>10</v>
       </c>
-      <c r="H7" s="103">
+      <c r="H7" s="115">
         <v>97</v>
       </c>
-      <c r="I7" s="103">
+      <c r="I7" s="115">
         <v>127</v>
       </c>
-      <c r="J7" s="103">
+      <c r="J7" s="115">
         <v>6</v>
       </c>
     </row>
@@ -4051,35 +4098,35 @@
       <c r="D8" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="104"/>
+      <c r="E8" s="116"/>
       <c r="F8" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="104"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116"/>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D9" s="59">
         <v>0.46533564814814815</v>
       </c>
-      <c r="E9" s="103">
+      <c r="E9" s="115">
         <v>3</v>
       </c>
       <c r="F9" s="61">
         <v>0.38201388888888888</v>
       </c>
-      <c r="G9" s="103">
+      <c r="G9" s="115">
         <v>1</v>
       </c>
-      <c r="H9" s="103">
+      <c r="H9" s="115">
         <v>157</v>
       </c>
-      <c r="I9" s="103">
+      <c r="I9" s="115">
         <v>467</v>
       </c>
-      <c r="J9" s="103">
+      <c r="J9" s="115">
         <v>2</v>
       </c>
     </row>
@@ -4087,35 +4134,35 @@
       <c r="D10" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E10" s="104"/>
+      <c r="E10" s="116"/>
       <c r="F10" s="55" t="s">
         <v>144</v>
       </c>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116"/>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D11" s="59">
         <v>0.46883101851851849</v>
       </c>
-      <c r="E11" s="103">
+      <c r="E11" s="115">
         <v>4</v>
       </c>
       <c r="F11" s="61">
         <v>0.38550925925925927</v>
       </c>
-      <c r="G11" s="103">
+      <c r="G11" s="115">
         <v>20</v>
       </c>
-      <c r="H11" s="103">
+      <c r="H11" s="115">
         <v>157</v>
       </c>
-      <c r="I11" s="103">
+      <c r="I11" s="115">
         <v>769</v>
       </c>
-      <c r="J11" s="103">
+      <c r="J11" s="115">
         <v>12</v>
       </c>
     </row>
@@ -4123,35 +4170,35 @@
       <c r="D12" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="104"/>
+      <c r="E12" s="116"/>
       <c r="F12" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
-      <c r="J12" s="104"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D13" s="59">
         <v>0.47228009259259257</v>
       </c>
-      <c r="E13" s="103">
+      <c r="E13" s="115">
         <v>5</v>
       </c>
       <c r="F13" s="61">
         <v>0.43062500000000004</v>
       </c>
-      <c r="G13" s="103">
+      <c r="G13" s="115">
         <v>19</v>
       </c>
-      <c r="H13" s="103">
+      <c r="H13" s="115">
         <v>179</v>
       </c>
-      <c r="I13" s="103">
+      <c r="I13" s="115">
         <v>1229</v>
       </c>
-      <c r="J13" s="103">
+      <c r="J13" s="115">
         <v>2</v>
       </c>
     </row>
@@ -4159,35 +4206,35 @@
       <c r="D14" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E14" s="104"/>
+      <c r="E14" s="116"/>
       <c r="F14" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116"/>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D15" s="59">
         <v>0.47574074074074074</v>
       </c>
-      <c r="E15" s="103">
+      <c r="E15" s="115">
         <v>6</v>
       </c>
       <c r="F15" s="61">
         <v>0.22575231481481481</v>
       </c>
-      <c r="G15" s="103">
+      <c r="G15" s="115">
         <v>12</v>
       </c>
-      <c r="H15" s="103">
+      <c r="H15" s="115">
         <v>73</v>
       </c>
-      <c r="I15" s="103">
+      <c r="I15" s="115">
         <v>101</v>
       </c>
-      <c r="J15" s="103">
+      <c r="J15" s="115">
         <v>4</v>
       </c>
     </row>
@@ -4195,35 +4242,35 @@
       <c r="D16" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="104"/>
+      <c r="E16" s="116"/>
       <c r="F16" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="G16" s="104"/>
-      <c r="H16" s="104"/>
-      <c r="I16" s="104"/>
-      <c r="J16" s="104"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="116"/>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D17" s="59">
         <v>0.47921296296296295</v>
       </c>
-      <c r="E17" s="103">
+      <c r="E17" s="115">
         <v>7</v>
       </c>
       <c r="F17" s="61">
         <v>0.47922453703703699</v>
       </c>
-      <c r="G17" s="103">
+      <c r="G17" s="115">
         <v>18</v>
       </c>
-      <c r="H17" s="103">
+      <c r="H17" s="115">
         <v>197</v>
       </c>
-      <c r="I17" s="103">
+      <c r="I17" s="115">
         <v>2221</v>
       </c>
-      <c r="J17" s="103">
+      <c r="J17" s="115">
         <v>4</v>
       </c>
     </row>
@@ -4231,35 +4278,35 @@
       <c r="D18" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="104"/>
+      <c r="E18" s="116"/>
       <c r="F18" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="G18" s="104"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="104"/>
-      <c r="J18" s="104"/>
+      <c r="G18" s="116"/>
+      <c r="H18" s="116"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="116"/>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D19" s="59">
         <v>0.48268518518518522</v>
       </c>
-      <c r="E19" s="103">
+      <c r="E19" s="115">
         <v>8</v>
       </c>
       <c r="F19" s="61">
         <v>0.14936342592592591</v>
       </c>
-      <c r="G19" s="103">
+      <c r="G19" s="115">
         <v>14</v>
       </c>
-      <c r="H19" s="103">
+      <c r="H19" s="115">
         <v>41</v>
       </c>
-      <c r="I19" s="103">
+      <c r="I19" s="115">
         <v>151</v>
       </c>
-      <c r="J19" s="103">
+      <c r="J19" s="115">
         <v>10</v>
       </c>
     </row>
@@ -4267,35 +4314,35 @@
       <c r="D20" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E20" s="104"/>
+      <c r="E20" s="116"/>
       <c r="F20" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="G20" s="104"/>
-      <c r="H20" s="104"/>
-      <c r="I20" s="104"/>
-      <c r="J20" s="104"/>
+      <c r="G20" s="116"/>
+      <c r="H20" s="116"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="116"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D21" s="59">
         <v>0.48616898148148152</v>
       </c>
-      <c r="E21" s="103">
+      <c r="E21" s="115">
         <v>9</v>
       </c>
       <c r="F21" s="61">
         <v>0.36118055555555556</v>
       </c>
-      <c r="G21" s="103">
+      <c r="G21" s="115">
         <v>21</v>
       </c>
-      <c r="H21" s="103">
+      <c r="H21" s="115">
         <v>137</v>
       </c>
-      <c r="I21" s="103">
+      <c r="I21" s="115">
         <v>179</v>
       </c>
-      <c r="J21" s="103">
+      <c r="J21" s="115">
         <v>2</v>
       </c>
     </row>
@@ -4303,35 +4350,35 @@
       <c r="D22" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E22" s="104"/>
+      <c r="E22" s="116"/>
       <c r="F22" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="G22" s="104"/>
-      <c r="H22" s="104"/>
-      <c r="I22" s="104"/>
-      <c r="J22" s="104"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="116"/>
+      <c r="I22" s="116"/>
+      <c r="J22" s="116"/>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D23" s="59">
         <v>0.48962962962962964</v>
       </c>
-      <c r="E23" s="103">
+      <c r="E23" s="115">
         <v>10</v>
       </c>
       <c r="F23" s="61">
         <v>0.48964120370370368</v>
       </c>
-      <c r="G23" s="103">
+      <c r="G23" s="115">
         <v>18</v>
       </c>
-      <c r="H23" s="103">
+      <c r="H23" s="115">
         <v>197</v>
       </c>
-      <c r="I23" s="103">
+      <c r="I23" s="115">
         <v>199</v>
       </c>
-      <c r="J23" s="103">
+      <c r="J23" s="115">
         <v>2</v>
       </c>
     </row>
@@ -4339,35 +4386,35 @@
       <c r="D24" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E24" s="104"/>
+      <c r="E24" s="116"/>
       <c r="F24" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="G24" s="104"/>
-      <c r="H24" s="104"/>
-      <c r="I24" s="104"/>
-      <c r="J24" s="104"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="116"/>
+      <c r="I24" s="116"/>
+      <c r="J24" s="116"/>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D25" s="59">
         <v>0.49311342592592594</v>
       </c>
-      <c r="E25" s="103">
+      <c r="E25" s="115">
         <v>11</v>
       </c>
       <c r="F25" s="61">
         <v>0.36812500000000004</v>
       </c>
-      <c r="G25" s="103">
+      <c r="G25" s="115">
         <v>21</v>
       </c>
-      <c r="H25" s="103">
+      <c r="H25" s="115">
         <v>137</v>
       </c>
-      <c r="I25" s="103">
+      <c r="I25" s="115">
         <v>223</v>
       </c>
-      <c r="J25" s="103">
+      <c r="J25" s="115">
         <v>8</v>
       </c>
     </row>
@@ -4375,35 +4422,35 @@
       <c r="D26" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="104"/>
+      <c r="E26" s="116"/>
       <c r="F26" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="G26" s="104"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="104"/>
-      <c r="J26" s="104"/>
+      <c r="G26" s="116"/>
+      <c r="H26" s="116"/>
+      <c r="I26" s="116"/>
+      <c r="J26" s="116"/>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D27" s="59">
         <v>0.49657407407407406</v>
       </c>
-      <c r="E27" s="103">
+      <c r="E27" s="115">
         <v>12</v>
       </c>
       <c r="F27" s="61">
         <v>7.9907407407407413E-2</v>
       </c>
-      <c r="G27" s="103">
+      <c r="G27" s="115">
         <v>16</v>
       </c>
-      <c r="H27" s="103">
+      <c r="H27" s="115">
         <v>11</v>
       </c>
-      <c r="I27" s="103">
+      <c r="I27" s="115">
         <v>263</v>
       </c>
-      <c r="J27" s="103">
+      <c r="J27" s="115">
         <v>2</v>
       </c>
     </row>
@@ -4411,35 +4458,35 @@
       <c r="D28" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E28" s="104"/>
+      <c r="E28" s="116"/>
       <c r="F28" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="G28" s="104"/>
-      <c r="H28" s="104"/>
-      <c r="I28" s="104"/>
-      <c r="J28" s="104"/>
+      <c r="G28" s="116"/>
+      <c r="H28" s="116"/>
+      <c r="I28" s="116"/>
+      <c r="J28" s="116"/>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D29" s="59">
         <v>0.50004629629629627</v>
       </c>
-      <c r="E29" s="103">
+      <c r="E29" s="115">
         <v>13</v>
       </c>
       <c r="F29" s="61">
         <v>0.25005787037037036</v>
       </c>
-      <c r="G29" s="103">
+      <c r="G29" s="115">
         <v>12</v>
       </c>
-      <c r="H29" s="103">
+      <c r="H29" s="115">
         <v>97</v>
       </c>
-      <c r="I29" s="103">
+      <c r="I29" s="115">
         <v>227</v>
       </c>
-      <c r="J29" s="103">
+      <c r="J29" s="115">
         <v>2</v>
       </c>
     </row>
@@ -4447,35 +4494,35 @@
       <c r="D30" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E30" s="104"/>
+      <c r="E30" s="116"/>
       <c r="F30" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="G30" s="104"/>
-      <c r="H30" s="104"/>
-      <c r="I30" s="104"/>
-      <c r="J30" s="104"/>
+      <c r="G30" s="116"/>
+      <c r="H30" s="116"/>
+      <c r="I30" s="116"/>
+      <c r="J30" s="116"/>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D31" s="59">
         <v>0.50004629629629627</v>
       </c>
-      <c r="E31" s="103">
+      <c r="E31" s="115">
         <v>14</v>
       </c>
       <c r="F31" s="61">
         <v>0.29172453703703705</v>
       </c>
-      <c r="G31" s="103">
+      <c r="G31" s="115">
         <v>10</v>
       </c>
-      <c r="H31" s="103">
+      <c r="H31" s="115">
         <v>109</v>
       </c>
-      <c r="I31" s="103">
+      <c r="I31" s="115">
         <v>269</v>
       </c>
-      <c r="J31" s="103">
+      <c r="J31" s="115">
         <v>4</v>
       </c>
     </row>
@@ -4483,35 +4530,35 @@
       <c r="D32" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E32" s="104"/>
+      <c r="E32" s="116"/>
       <c r="F32" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="G32" s="104"/>
-      <c r="H32" s="104"/>
-      <c r="I32" s="104"/>
-      <c r="J32" s="104"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="116"/>
+      <c r="I32" s="116"/>
+      <c r="J32" s="116"/>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D33" s="59">
         <v>0.50004629629629627</v>
       </c>
-      <c r="E33" s="103">
+      <c r="E33" s="115">
         <v>15</v>
       </c>
       <c r="F33" s="61">
         <v>8.3391203703703717E-2</v>
       </c>
-      <c r="G33" s="103">
+      <c r="G33" s="115">
         <v>16</v>
       </c>
-      <c r="H33" s="103">
+      <c r="H33" s="115">
         <v>23</v>
       </c>
-      <c r="I33" s="103">
+      <c r="I33" s="115">
         <v>59</v>
       </c>
-      <c r="J33" s="103">
+      <c r="J33" s="115">
         <v>2</v>
       </c>
     </row>
@@ -4519,35 +4566,35 @@
       <c r="D34" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E34" s="104"/>
+      <c r="E34" s="116"/>
       <c r="F34" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="G34" s="104"/>
-      <c r="H34" s="104"/>
-      <c r="I34" s="104"/>
-      <c r="J34" s="104"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="116"/>
+      <c r="J34" s="116"/>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D35" s="59">
         <v>0.50012731481481476</v>
       </c>
-      <c r="E35" s="103">
+      <c r="E35" s="115">
         <v>16</v>
       </c>
       <c r="F35" s="61">
         <v>0.33347222222222223</v>
       </c>
-      <c r="G35" s="103">
+      <c r="G35" s="115">
         <v>22</v>
       </c>
-      <c r="H35" s="103">
+      <c r="H35" s="115">
         <v>137</v>
       </c>
-      <c r="I35" s="103">
+      <c r="I35" s="115">
         <v>313</v>
       </c>
-      <c r="J35" s="103">
+      <c r="J35" s="115">
         <v>8</v>
       </c>
     </row>
@@ -4555,35 +4602,35 @@
       <c r="D36" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E36" s="104"/>
+      <c r="E36" s="116"/>
       <c r="F36" s="55" t="s">
         <v>151</v>
       </c>
-      <c r="G36" s="104"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="104"/>
-      <c r="J36" s="104"/>
+      <c r="G36" s="116"/>
+      <c r="H36" s="116"/>
+      <c r="I36" s="116"/>
+      <c r="J36" s="116"/>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D37" s="59">
         <v>0.50005787037037031</v>
       </c>
-      <c r="E37" s="103">
+      <c r="E37" s="115">
         <v>17</v>
       </c>
       <c r="F37" s="61">
         <v>0.12508101851851852</v>
       </c>
-      <c r="G37" s="103">
+      <c r="G37" s="115">
         <v>15</v>
       </c>
-      <c r="H37" s="103">
+      <c r="H37" s="115">
         <v>41</v>
       </c>
-      <c r="I37" s="103">
+      <c r="I37" s="115">
         <v>97</v>
       </c>
-      <c r="J37" s="103">
+      <c r="J37" s="115">
         <v>8</v>
       </c>
     </row>
@@ -4591,102 +4638,102 @@
       <c r="D38" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="E38" s="104"/>
+      <c r="E38" s="116"/>
       <c r="F38" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="104"/>
-      <c r="H38" s="104"/>
-      <c r="I38" s="104"/>
-      <c r="J38" s="104"/>
+      <c r="G38" s="116"/>
+      <c r="H38" s="116"/>
+      <c r="I38" s="116"/>
+      <c r="J38" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4719,10 +4766,10 @@
       </c>
     </row>
     <row r="18" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="105" t="s">
+      <c r="J18" s="117" t="s">
         <v>115</v>
       </c>
-      <c r="K18" s="105" t="s">
+      <c r="K18" s="117" t="s">
         <v>116</v>
       </c>
       <c r="L18" s="6" t="s">
@@ -4730,8 +4777,8 @@
       </c>
     </row>
     <row r="19" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J19" s="105"/>
-      <c r="K19" s="105"/>
+      <c r="J19" s="117"/>
+      <c r="K19" s="117"/>
       <c r="L19" s="6" t="s">
         <v>139</v>
       </c>
@@ -4945,40 +4992,42 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:K15"/>
+  <dimension ref="D4:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="119" t="s">
+      <c r="D5" s="118" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="116">
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="79">
         <v>0.62883101851851853</v>
       </c>
-      <c r="H5" s="115"/>
+      <c r="H5" s="78"/>
     </row>
     <row r="6" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="E6" s="102"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="118">
+      <c r="E6" s="114"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="80">
         <v>478</v>
       </c>
-      <c r="H6" s="115"/>
+      <c r="H6" s="78"/>
     </row>
     <row r="7" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="30" t="s">
@@ -4990,26 +5039,26 @@
       <c r="F7" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="127" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="107"/>
-      <c r="J7" s="106" t="s">
+      <c r="H7" s="73"/>
+      <c r="J7" s="72" t="s">
         <v>167</v>
       </c>
-      <c r="K7" s="106"/>
+      <c r="K7" s="72"/>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D8" s="122" t="s">
+      <c r="D8" s="82" t="s">
         <v>156</v>
       </c>
-      <c r="E8" s="121">
+      <c r="E8" s="81">
         <v>55</v>
       </c>
-      <c r="F8" s="122" t="s">
+      <c r="F8" s="82" t="s">
         <v>169</v>
       </c>
-      <c r="G8" s="120" t="b">
+      <c r="G8" s="125" t="b">
         <f>E$7&lt; E8</f>
         <v>1</v>
       </c>
@@ -5023,10 +5072,10 @@
         <v>49</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="G9" s="4" t="b">
-        <f t="shared" ref="G9:G12" si="0">E$7&lt; E9</f>
+        <v>171</v>
+      </c>
+      <c r="G9" s="126" t="b">
+        <f t="shared" ref="G9:G13" si="0">E$7&lt; E9</f>
         <v>1</v>
       </c>
       <c r="H9" s="63"/>
@@ -5039,9 +5088,9 @@
         <v>104</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="G10" s="4" t="b">
+        <v>172</v>
+      </c>
+      <c r="G10" s="126" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -5055,9 +5104,9 @@
         <v>495</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="G11" s="4" t="b">
+        <v>173</v>
+      </c>
+      <c r="G11" s="126" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -5071,50 +5120,64 @@
         <v>2695</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" s="4" t="b">
+        <v>174</v>
+      </c>
+      <c r="G12" s="126" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H12" s="63"/>
     </row>
-    <row r="13" spans="4:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D13" s="113"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="17" t="s">
+    <row r="13" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="122" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="31">
+        <f>G6-E7</f>
+        <v>442</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="123"/>
+      <c r="H13" s="71"/>
+    </row>
+    <row r="14" spans="4:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="120"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="G13" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="108" t="s">
+      <c r="G14" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="90" t="s">
+      <c r="E15" s="102" t="s">
         <v>162</v>
       </c>
-      <c r="F14" s="90"/>
-      <c r="G14" s="91"/>
-    </row>
-    <row r="15" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="109" t="s">
+      <c r="F15" s="102"/>
+      <c r="G15" s="103"/>
+    </row>
+    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="124" t="s">
         <v>165</v>
       </c>
-      <c r="E15" s="112">
+      <c r="E16" s="77">
         <v>263</v>
       </c>
-      <c r="F15" s="110"/>
-      <c r="G15" s="111"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>